<commit_message>
Updated Pokédex file and testing evos
</commit_message>
<xml_diff>
--- a/Pokedex.xlsx
+++ b/Pokedex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlos_vasquez/Desktop/CS/2 Fall 2023/Shell/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9790EC-CBE7-CF4F-9C5A-6C57C6E7F1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494B6A50-8F78-564E-B8FB-19852E3B0D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9280" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{C6720D87-1F10-3A4F-84A9-DA5238F3465E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{C6720D87-1F10-3A4F-84A9-DA5238F3465E}"/>
   </bookViews>
   <sheets>
     <sheet name="National" sheetId="3" r:id="rId1"/>
@@ -925,12 +925,6 @@
     <t>Trade with King's Rock</t>
   </si>
   <si>
-    <t>Pokémon</t>
-  </si>
-  <si>
-    <t>Brahches</t>
-  </si>
-  <si>
     <t>Level req</t>
   </si>
   <si>
@@ -944,6 +938,12 @@
   </si>
   <si>
     <t>Method(s)</t>
+  </si>
+  <si>
+    <t>Happiness</t>
+  </si>
+  <si>
+    <t>Branches</t>
   </si>
 </sst>
 </file>
@@ -1314,9 +1314,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCA7907-3604-4B47-A2AF-98FA510591CC}">
   <dimension ref="A1:H252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1351,7 +1351,7 @@
         <v>290</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2134,7 +2134,7 @@
         <v>194</v>
       </c>
       <c r="H43" t="s">
-        <v>277</v>
+        <v>299</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -3386,7 +3386,7 @@
         <v>267</v>
       </c>
       <c r="H114" t="s">
-        <v>277</v>
+        <v>299</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
@@ -4380,7 +4380,7 @@
         <v>28</v>
       </c>
       <c r="H173" t="s">
-        <v>277</v>
+        <v>299</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
@@ -4400,7 +4400,7 @@
         <v>36</v>
       </c>
       <c r="H174" t="s">
-        <v>277</v>
+        <v>299</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
@@ -4423,7 +4423,7 @@
         <v>40</v>
       </c>
       <c r="H175" t="s">
-        <v>277</v>
+        <v>299</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
@@ -4446,7 +4446,7 @@
         <v>201</v>
       </c>
       <c r="H176" t="s">
-        <v>277</v>
+        <v>299</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
@@ -5637,8 +5637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB7BF82-EA9E-FB47-B306-E94399F11581}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5648,13 +5648,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>296</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>174</v>
@@ -5786,7 +5786,7 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E13" t="s">
         <v>107</v>
@@ -5794,7 +5794,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E14" t="s">
         <v>108</v>
@@ -5802,7 +5802,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E15" t="s">
         <v>262</v>

</xml_diff>

<commit_message>
Updated Pokedex file and figured branch evos
</commit_message>
<xml_diff>
--- a/Pokedex.xlsx
+++ b/Pokedex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlos_vasquez/Desktop/CS/2 Fall 2023/Shell/pokedex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D57183-24EB-BA4D-9DC2-365E12911E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65F6636-5C15-D14D-9BF3-FA8919A7C8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{C6720D87-1F10-3A4F-84A9-DA5238F3465E}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2920" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2920" uniqueCount="303">
   <si>
     <t>Bulbasaur</t>
   </si>
@@ -944,6 +944,12 @@
   </si>
   <si>
     <t>Level</t>
+  </si>
+  <si>
+    <t>Happiness during Night</t>
+  </si>
+  <si>
+    <t>Happiness during Day</t>
   </si>
 </sst>
 </file>
@@ -1316,7 +1322,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5638,7 +5644,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5761,7 +5767,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="E11" t="s">
         <v>221</v>
@@ -5769,7 +5775,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
-        <v>288</v>
+        <v>301</v>
       </c>
       <c r="E12" t="s">
         <v>222</v>

</xml_diff>

<commit_message>
Updated Dex file, added typing, streamlined code
</commit_message>
<xml_diff>
--- a/Pokedex.xlsx
+++ b/Pokedex.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlos_vasquez/Desktop/CS/2 Fall 2023/Shell/pokedex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65F6636-5C15-D14D-9BF3-FA8919A7C8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D516A4-BCC0-5847-AA8B-A85182235F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{C6720D87-1F10-3A4F-84A9-DA5238F3465E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{C6720D87-1F10-3A4F-84A9-DA5238F3465E}"/>
   </bookViews>
   <sheets>
     <sheet name="National" sheetId="3" r:id="rId1"/>
     <sheet name="Branch Evos" sheetId="6" r:id="rId2"/>
-    <sheet name="Generation1" sheetId="1" r:id="rId3"/>
-    <sheet name="Generation2" sheetId="2" r:id="rId4"/>
-    <sheet name="Generation2 (2)" sheetId="4" r:id="rId5"/>
-    <sheet name="National (2)" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId3"/>
+    <sheet name="Generation1" sheetId="1" r:id="rId4"/>
+    <sheet name="Generation2" sheetId="2" r:id="rId5"/>
+    <sheet name="Generation2 (2)" sheetId="4" r:id="rId6"/>
+    <sheet name="National (2)" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2920" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2956" uniqueCount="305">
   <si>
     <t>Bulbasaur</t>
   </si>
@@ -934,9 +935,6 @@
     <t>Attack = Defense</t>
   </si>
   <si>
-    <t>Method(s)</t>
-  </si>
-  <si>
     <t>Happiness</t>
   </si>
   <si>
@@ -950,6 +948,15 @@
   </si>
   <si>
     <t>Happiness during Day</t>
+  </si>
+  <si>
+    <t>Means</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Attacking</t>
   </si>
 </sst>
 </file>
@@ -1320,9 +1327,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCA7907-3604-4B47-A2AF-98FA510591CC}">
   <dimension ref="A1:H252"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E130" sqref="E130"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1357,7 +1364,7 @@
         <v>290</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2016,9 +2023,6 @@
       <c r="F37" t="s">
         <v>36</v>
       </c>
-      <c r="G37" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
@@ -2140,7 +2144,7 @@
         <v>194</v>
       </c>
       <c r="H43" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -3392,7 +3396,7 @@
         <v>267</v>
       </c>
       <c r="H114" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
@@ -4386,7 +4390,7 @@
         <v>28</v>
       </c>
       <c r="H173" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
@@ -4406,7 +4410,7 @@
         <v>36</v>
       </c>
       <c r="H174" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
@@ -4429,7 +4433,7 @@
         <v>40</v>
       </c>
       <c r="H175" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
@@ -4452,7 +4456,7 @@
         <v>201</v>
       </c>
       <c r="H176" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
@@ -5643,13 +5647,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB7BF82-EA9E-FB47-B306-E94399F11581}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -5660,125 +5664,125 @@
         <v>299</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>173</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
         <v>283</v>
-      </c>
-      <c r="E2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E3" t="s">
         <v>284</v>
-      </c>
-      <c r="E3" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>62</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" t="s">
         <v>279</v>
-      </c>
-      <c r="E4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E5" t="s">
         <v>293</v>
-      </c>
-      <c r="E5" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>80</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6">
         <v>37</v>
-      </c>
-      <c r="E6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
+        <v>224</v>
+      </c>
+      <c r="E7" t="s">
         <v>293</v>
-      </c>
-      <c r="E7" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>134</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>5</v>
       </c>
       <c r="D8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" t="s">
         <v>279</v>
-      </c>
-      <c r="E8" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" t="s">
         <v>280</v>
-      </c>
-      <c r="E9" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" t="s">
         <v>281</v>
-      </c>
-      <c r="E10" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
-        <v>302</v>
+        <v>221</v>
       </c>
       <c r="E11" t="s">
-        <v>221</v>
+        <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
-        <v>301</v>
+        <v>222</v>
       </c>
       <c r="E12" t="s">
-        <v>222</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -5786,32 +5790,32 @@
         <v>261</v>
       </c>
       <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13">
         <v>3</v>
       </c>
-      <c r="C13">
-        <v>20</v>
-      </c>
       <c r="D13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" t="s">
         <v>294</v>
-      </c>
-      <c r="E13" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" t="s">
         <v>295</v>
-      </c>
-      <c r="E14" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
+        <v>262</v>
+      </c>
+      <c r="E15" t="s">
         <v>296</v>
-      </c>
-      <c r="E15" t="s">
-        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -5820,6 +5824,533 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D70D5D-189C-114A-AA66-3EAEA4D4DAFA}">
+  <dimension ref="A1:S20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:S1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="N3">
+        <v>0.5</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>0.5</v>
+      </c>
+      <c r="P4">
+        <v>0.5</v>
+      </c>
+      <c r="R4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+      <c r="F5">
+        <v>0.5</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+      <c r="F6">
+        <v>0.5</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="I7">
+        <v>0.5</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>0.5</v>
+      </c>
+      <c r="M7">
+        <v>0.5</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>0.5</v>
+      </c>
+      <c r="R7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>0.5</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
+      <c r="R8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>0.5</v>
+      </c>
+      <c r="K9">
+        <v>0.5</v>
+      </c>
+      <c r="L9">
+        <v>0.5</v>
+      </c>
+      <c r="M9">
+        <v>0.5</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>2</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+      <c r="S9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>0.5</v>
+      </c>
+      <c r="J10">
+        <v>0.5</v>
+      </c>
+      <c r="N10">
+        <v>0.5</v>
+      </c>
+      <c r="O10">
+        <v>0.5</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>0.5</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0.5</v>
+      </c>
+      <c r="N11">
+        <v>2</v>
+      </c>
+      <c r="R11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12">
+        <v>0.5</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>0.5</v>
+      </c>
+      <c r="R12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>0.5</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>0.5</v>
+      </c>
+      <c r="I14">
+        <v>0.5</v>
+      </c>
+      <c r="K14">
+        <v>0.5</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>0.5</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="R14">
+        <v>0.5</v>
+      </c>
+      <c r="S14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>0.5</v>
+      </c>
+      <c r="J15">
+        <v>0.5</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="R15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="Q16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="P17">
+        <v>2</v>
+      </c>
+      <c r="R17">
+        <v>0.5</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="H18">
+        <v>0.5</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>0.5</v>
+      </c>
+      <c r="S18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19">
+        <v>0.5</v>
+      </c>
+      <c r="D19">
+        <v>0.5</v>
+      </c>
+      <c r="E19">
+        <v>0.5</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="R19">
+        <v>0.5</v>
+      </c>
+      <c r="S19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20">
+        <v>0.5</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>0.5</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <v>2</v>
+      </c>
+      <c r="R20">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93843203-7973-1746-84FC-CFCCAE980FCE}">
   <dimension ref="A1:G153"/>
   <sheetViews>
@@ -9342,7 +9873,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3613162D-3AD3-594F-BD4F-A41FCE043DF4}">
   <dimension ref="A1:G101"/>
   <sheetViews>
@@ -10919,7 +11450,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B2C876-5489-8A4D-BC72-1A109E9B4968}">
   <dimension ref="A1:G101"/>
   <sheetViews>
@@ -12508,7 +13039,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F07C246-D3A7-7F45-962C-E17945F837A4}">
   <dimension ref="A1:G153"/>
   <sheetViews>

</xml_diff>